<commit_message>
03/07/2024 fin de journée SCB
</commit_message>
<xml_diff>
--- a/tests/fichier_test/e_e_p.xlsx
+++ b/tests/fichier_test/e_e_p.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet SCB\Project\reHabi\tests\fichier_test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Feuil1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -517,387 +522,386 @@
     <t>2022-05-17 18:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">PROF016	Marketing
+    <t>PROF029</t>
+  </si>
+  <si>
+    <t>Don</t>
+  </si>
+  <si>
+    <t>D56851</t>
+  </si>
+  <si>
+    <t>P010</t>
+  </si>
+  <si>
+    <t>Communications Manager</t>
+  </si>
+  <si>
+    <t>2003-02-16 08:00:00</t>
+  </si>
+  <si>
+    <t>ENT006</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>PROF015</t>
+  </si>
+  <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>E65420</t>
+  </si>
+  <si>
+    <t>P011</t>
+  </si>
+  <si>
+    <t>IT Technician</t>
+  </si>
+  <si>
+    <t>Fritz</t>
+  </si>
+  <si>
+    <t>F65787</t>
+  </si>
+  <si>
+    <t>P012</t>
+  </si>
+  <si>
+    <t>Help Desk Specialist</t>
+  </si>
+  <si>
+    <t>2010-01-29 08:00:00</t>
+  </si>
+  <si>
+    <t>Gael</t>
+  </si>
+  <si>
+    <t>G78427</t>
+  </si>
+  <si>
+    <t>Social Media Manager</t>
+  </si>
+  <si>
+    <t>2014-05-15 08:00:00</t>
+  </si>
+  <si>
+    <t>PROF017</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>H64223</t>
+  </si>
+  <si>
+    <t>P013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT Support </t>
+  </si>
+  <si>
+    <t>2020-11-17 08:00:00</t>
+  </si>
+  <si>
+    <t>PROF018</t>
+  </si>
+  <si>
+    <t>Illan</t>
+  </si>
+  <si>
+    <t>I673219</t>
+  </si>
+  <si>
+    <t>P014</t>
+  </si>
+  <si>
+    <t>Help Desk Technician</t>
+  </si>
+  <si>
+    <t>2016-03-06 08:00:00</t>
+  </si>
+  <si>
+    <t>PROF019</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>J09386</t>
+  </si>
+  <si>
+    <t>P015</t>
+  </si>
+  <si>
+    <t>IT Administrator</t>
+  </si>
+  <si>
+    <t>Kreold</t>
+  </si>
+  <si>
+    <t>K34577</t>
+  </si>
+  <si>
+    <t>P016</t>
+  </si>
+  <si>
+    <t>Communications Specialist</t>
+  </si>
+  <si>
+    <t>PROF021</t>
+  </si>
+  <si>
+    <t>Landry</t>
+  </si>
+  <si>
+    <t>L25678</t>
+  </si>
+  <si>
+    <t>P017</t>
+  </si>
+  <si>
+    <t>IT Analyst</t>
+  </si>
+  <si>
+    <t>2016-12-16 08:00:00</t>
+  </si>
+  <si>
+    <t>PROF022</t>
+  </si>
+  <si>
+    <t>Maelle</t>
+  </si>
+  <si>
+    <t>M08007</t>
+  </si>
+  <si>
+    <t>P018</t>
+  </si>
+  <si>
+    <t>Senior Help Desk Technician</t>
+  </si>
+  <si>
+    <t>2014-09-10 08:00:00</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>N89321</t>
+  </si>
+  <si>
+    <t>P019</t>
+  </si>
+  <si>
+    <t>Public Relations Manager</t>
+  </si>
+  <si>
+    <t>2020-12-16 10:00:00</t>
+  </si>
+  <si>
+    <t>PROF024</t>
+  </si>
+  <si>
+    <t>OLO</t>
+  </si>
+  <si>
+    <t>O07866</t>
+  </si>
+  <si>
+    <t>P020</t>
+  </si>
+  <si>
+    <t>Network Administrator</t>
+  </si>
+  <si>
+    <t>2014-02-06 08:00:00</t>
+  </si>
+  <si>
+    <t>PROF025</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>P73573</t>
+  </si>
+  <si>
+    <t>P021</t>
+  </si>
+  <si>
+    <t>Desktop Support</t>
+  </si>
+  <si>
+    <t>2020-08-16 10:50:10</t>
+  </si>
+  <si>
+    <t>PROF026</t>
+  </si>
+  <si>
+    <t>Qualvin</t>
+  </si>
+  <si>
+    <t>Q87382</t>
+  </si>
+  <si>
+    <t>P022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systems Engineer </t>
+  </si>
+  <si>
+    <t>PROF027</t>
+  </si>
+  <si>
+    <t>Roland</t>
+  </si>
+  <si>
+    <t>R8729</t>
+  </si>
+  <si>
+    <t>P023</t>
+  </si>
+  <si>
+    <t>Marketing Coordinator</t>
+  </si>
+  <si>
+    <t>2014-08-26 13:40:00</t>
+  </si>
+  <si>
+    <t>Sabail</t>
+  </si>
+  <si>
+    <t>S848726</t>
+  </si>
+  <si>
+    <t>P024</t>
+  </si>
+  <si>
+    <t>Database Administrator</t>
+  </si>
+  <si>
+    <t>Tristan</t>
+  </si>
+  <si>
+    <t>T48237</t>
+  </si>
+  <si>
+    <t>P025</t>
+  </si>
+  <si>
+    <t>Technical Support</t>
+  </si>
+  <si>
+    <t>1999-08-16 08:09:00</t>
+  </si>
+  <si>
+    <t>Ugo</t>
+  </si>
+  <si>
+    <t>U87183</t>
+  </si>
+  <si>
+    <t>P026</t>
+  </si>
+  <si>
+    <t>Community Manager</t>
+  </si>
+  <si>
+    <t>2001-08-16 08:40:00</t>
+  </si>
+  <si>
+    <t>Valère</t>
+  </si>
+  <si>
+    <t>V40419</t>
+  </si>
+  <si>
+    <t>P027</t>
+  </si>
+  <si>
+    <t>IT Consultant</t>
+  </si>
+  <si>
+    <t>Wihtney</t>
+  </si>
+  <si>
+    <t>W8136</t>
+  </si>
+  <si>
+    <t>P028</t>
+  </si>
+  <si>
+    <t>Help Desk Manager</t>
+  </si>
+  <si>
+    <t>2007-07-04 08:00:00</t>
+  </si>
+  <si>
+    <t>Xillac</t>
+  </si>
+  <si>
+    <t>X562314</t>
+  </si>
+  <si>
+    <t>P029</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>2011-04-23 08:00:00</t>
+  </si>
+  <si>
+    <t>PROF034</t>
+  </si>
+  <si>
+    <t>Yacine</t>
+  </si>
+  <si>
+    <t>Y019897</t>
+  </si>
+  <si>
+    <t>P030</t>
+  </si>
+  <si>
+    <t>PR Specialist</t>
+  </si>
+  <si>
+    <t>PROF035</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Z80900</t>
+  </si>
+  <si>
+    <t>P031</t>
+  </si>
+  <si>
+    <t>IT Security Analyst</t>
+  </si>
+  <si>
+    <t>2019-06-03 08:00:00</t>
+  </si>
+  <si>
+    <t>2021-11-18 15:10:00</t>
+  </si>
+  <si>
+    <t>PROF036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROF016
 </t>
-  </si>
-  <si>
-    <t>PROF029</t>
-  </si>
-  <si>
-    <t>Don</t>
-  </si>
-  <si>
-    <t>D56851</t>
-  </si>
-  <si>
-    <t>P010</t>
-  </si>
-  <si>
-    <t>Communications Manager</t>
-  </si>
-  <si>
-    <t>2003-02-16 08:00:00</t>
-  </si>
-  <si>
-    <t>ENT006</t>
-  </si>
-  <si>
-    <t>Communications</t>
-  </si>
-  <si>
-    <t>PROF015</t>
-  </si>
-  <si>
-    <t>Eli</t>
-  </si>
-  <si>
-    <t>E65420</t>
-  </si>
-  <si>
-    <t>P011</t>
-  </si>
-  <si>
-    <t>IT Technician</t>
-  </si>
-  <si>
-    <t>Fritz</t>
-  </si>
-  <si>
-    <t>F65787</t>
-  </si>
-  <si>
-    <t>P012</t>
-  </si>
-  <si>
-    <t>Help Desk Specialist</t>
-  </si>
-  <si>
-    <t>2010-01-29 08:00:00</t>
-  </si>
-  <si>
-    <t>Gael</t>
-  </si>
-  <si>
-    <t>G78427</t>
-  </si>
-  <si>
-    <t>Social Media Manager</t>
-  </si>
-  <si>
-    <t>2014-05-15 08:00:00</t>
-  </si>
-  <si>
-    <t>PROF017</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>H64223</t>
-  </si>
-  <si>
-    <t>P013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT Support </t>
-  </si>
-  <si>
-    <t>2020-11-17 08:00:00</t>
-  </si>
-  <si>
-    <t>PROF018</t>
-  </si>
-  <si>
-    <t>Illan</t>
-  </si>
-  <si>
-    <t>I673219</t>
-  </si>
-  <si>
-    <t>P014</t>
-  </si>
-  <si>
-    <t>Help Desk Technician</t>
-  </si>
-  <si>
-    <t>2016-03-06 08:00:00</t>
-  </si>
-  <si>
-    <t>PROF019</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>J09386</t>
-  </si>
-  <si>
-    <t>P015</t>
-  </si>
-  <si>
-    <t>IT Administrator</t>
-  </si>
-  <si>
-    <t>Kreold</t>
-  </si>
-  <si>
-    <t>K34577</t>
-  </si>
-  <si>
-    <t>P016</t>
-  </si>
-  <si>
-    <t>Communications Specialist</t>
-  </si>
-  <si>
-    <t>PROF021</t>
-  </si>
-  <si>
-    <t>Landry</t>
-  </si>
-  <si>
-    <t>L25678</t>
-  </si>
-  <si>
-    <t>P017</t>
-  </si>
-  <si>
-    <t>IT Analyst</t>
-  </si>
-  <si>
-    <t>2016-12-16 08:00:00</t>
-  </si>
-  <si>
-    <t>PROF022</t>
-  </si>
-  <si>
-    <t>Maelle</t>
-  </si>
-  <si>
-    <t>M08007</t>
-  </si>
-  <si>
-    <t>P018</t>
-  </si>
-  <si>
-    <t>Senior Help Desk Technician</t>
-  </si>
-  <si>
-    <t>2014-09-10 08:00:00</t>
-  </si>
-  <si>
-    <t>Nathan</t>
-  </si>
-  <si>
-    <t>N89321</t>
-  </si>
-  <si>
-    <t>P019</t>
-  </si>
-  <si>
-    <t>Public Relations Manager</t>
-  </si>
-  <si>
-    <t>2020-12-16 10:00:00</t>
-  </si>
-  <si>
-    <t>PROF024</t>
-  </si>
-  <si>
-    <t>OLO</t>
-  </si>
-  <si>
-    <t>O07866</t>
-  </si>
-  <si>
-    <t>P020</t>
-  </si>
-  <si>
-    <t>Network Administrator</t>
-  </si>
-  <si>
-    <t>2014-02-06 08:00:00</t>
-  </si>
-  <si>
-    <t>PROF025</t>
-  </si>
-  <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>P73573</t>
-  </si>
-  <si>
-    <t>P021</t>
-  </si>
-  <si>
-    <t>Desktop Support</t>
-  </si>
-  <si>
-    <t>2020-08-16 10:50:10</t>
-  </si>
-  <si>
-    <t>PROF026</t>
-  </si>
-  <si>
-    <t>Qualvin</t>
-  </si>
-  <si>
-    <t>Q87382</t>
-  </si>
-  <si>
-    <t>P022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systems Engineer </t>
-  </si>
-  <si>
-    <t>PROF027</t>
-  </si>
-  <si>
-    <t>Roland</t>
-  </si>
-  <si>
-    <t>R8729</t>
-  </si>
-  <si>
-    <t>P023</t>
-  </si>
-  <si>
-    <t>Marketing Coordinator</t>
-  </si>
-  <si>
-    <t>2014-08-26 13:40:00</t>
-  </si>
-  <si>
-    <t>Sabail</t>
-  </si>
-  <si>
-    <t>S848726</t>
-  </si>
-  <si>
-    <t>P024</t>
-  </si>
-  <si>
-    <t>Database Administrator</t>
-  </si>
-  <si>
-    <t>Tristan</t>
-  </si>
-  <si>
-    <t>T48237</t>
-  </si>
-  <si>
-    <t>P025</t>
-  </si>
-  <si>
-    <t>Technical Support</t>
-  </si>
-  <si>
-    <t>1999-08-16 08:09:00</t>
-  </si>
-  <si>
-    <t>Ugo</t>
-  </si>
-  <si>
-    <t>U87183</t>
-  </si>
-  <si>
-    <t>P026</t>
-  </si>
-  <si>
-    <t>Community Manager</t>
-  </si>
-  <si>
-    <t>2001-08-16 08:40:00</t>
-  </si>
-  <si>
-    <t>Valère</t>
-  </si>
-  <si>
-    <t>V40419</t>
-  </si>
-  <si>
-    <t>P027</t>
-  </si>
-  <si>
-    <t>IT Consultant</t>
-  </si>
-  <si>
-    <t>Wihtney</t>
-  </si>
-  <si>
-    <t>W8136</t>
-  </si>
-  <si>
-    <t>P028</t>
-  </si>
-  <si>
-    <t>Help Desk Manager</t>
-  </si>
-  <si>
-    <t>2007-07-04 08:00:00</t>
-  </si>
-  <si>
-    <t>Xillac</t>
-  </si>
-  <si>
-    <t>X562314</t>
-  </si>
-  <si>
-    <t>P029</t>
-  </si>
-  <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
-    <t>2011-04-23 08:00:00</t>
-  </si>
-  <si>
-    <t>PROF034</t>
-  </si>
-  <si>
-    <t>Yacine</t>
-  </si>
-  <si>
-    <t>Y019897</t>
-  </si>
-  <si>
-    <t>P030</t>
-  </si>
-  <si>
-    <t>PR Specialist</t>
-  </si>
-  <si>
-    <t>PROF035</t>
-  </si>
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Z80900</t>
-  </si>
-  <si>
-    <t>P031</t>
-  </si>
-  <si>
-    <t>IT Security Analyst</t>
-  </si>
-  <si>
-    <t>2019-06-03 08:00:00</t>
-  </si>
-  <si>
-    <t>2021-11-18 15:10:00</t>
-  </si>
-  <si>
-    <t>PROF036</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -954,43 +958,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1001,10 +1008,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1042,71 +1049,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,7 +1141,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1157,11 +1164,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1170,13 +1177,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1186,7 +1193,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1195,7 +1202,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1204,7 +1211,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1212,10 +1219,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1286,28 +1293,30 @@
   </sheetPr>
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="21.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="26.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="21.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="21.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="30.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1361,7 @@
       </c>
       <c r="O1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1393,7 +1402,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1434,7 +1443,7 @@
       </c>
       <c r="O3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1475,7 +1484,7 @@
       </c>
       <c r="O4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1525,7 @@
       </c>
       <c r="O5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1559,7 +1568,7 @@
       </c>
       <c r="O6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1602,7 +1611,7 @@
       </c>
       <c r="O7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -1645,7 +1654,7 @@
       </c>
       <c r="O8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -1688,7 +1697,7 @@
       </c>
       <c r="O9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1731,7 +1740,7 @@
       </c>
       <c r="O10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1772,7 +1781,7 @@
       </c>
       <c r="O11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -1813,7 +1822,7 @@
       </c>
       <c r="O12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="13" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
@@ -1854,7 +1863,7 @@
       </c>
       <c r="O13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>58</v>
       </c>
@@ -1895,7 +1904,7 @@
       </c>
       <c r="O14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
@@ -1936,7 +1945,7 @@
       </c>
       <c r="O15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>58</v>
       </c>
@@ -1977,7 +1986,7 @@
       </c>
       <c r="O16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -2018,7 +2027,7 @@
       </c>
       <c r="O17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>64</v>
       </c>
@@ -2059,7 +2068,7 @@
       </c>
       <c r="O18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="19" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>69</v>
       </c>
@@ -2100,7 +2109,7 @@
       </c>
       <c r="O19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>74</v>
       </c>
@@ -2141,7 +2150,7 @@
       </c>
       <c r="O20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
@@ -2182,7 +2191,7 @@
       </c>
       <c r="O21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>80</v>
       </c>
@@ -2223,7 +2232,7 @@
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>83</v>
       </c>
@@ -2264,7 +2273,7 @@
       </c>
       <c r="O23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>88</v>
       </c>
@@ -2305,7 +2314,7 @@
       </c>
       <c r="O24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>91</v>
       </c>
@@ -2346,7 +2355,7 @@
       </c>
       <c r="O25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>94</v>
       </c>
@@ -2387,7 +2396,7 @@
       </c>
       <c r="O26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>98</v>
       </c>
@@ -2428,7 +2437,7 @@
       </c>
       <c r="O27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>101</v>
       </c>
@@ -2469,7 +2478,7 @@
       </c>
       <c r="O28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>105</v>
       </c>
@@ -2512,7 +2521,7 @@
       </c>
       <c r="O29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>109</v>
       </c>
@@ -2553,7 +2562,7 @@
       </c>
       <c r="O30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>114</v>
       </c>
@@ -2594,7 +2603,7 @@
       </c>
       <c r="O31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>117</v>
       </c>
@@ -2635,7 +2644,7 @@
       </c>
       <c r="O32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="33" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>117</v>
       </c>
@@ -2676,7 +2685,7 @@
       </c>
       <c r="O33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="34" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>117</v>
       </c>
@@ -2717,7 +2726,7 @@
       </c>
       <c r="O34" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="35" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>123</v>
       </c>
@@ -2758,7 +2767,7 @@
       </c>
       <c r="O35" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="36" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>127</v>
       </c>
@@ -2799,7 +2808,7 @@
       </c>
       <c r="O36" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="37" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>130</v>
       </c>
@@ -2840,7 +2849,7 @@
       </c>
       <c r="O37" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="38" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>135</v>
       </c>
@@ -2881,7 +2890,7 @@
       </c>
       <c r="O38" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="39" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>135</v>
       </c>
@@ -2922,7 +2931,7 @@
       </c>
       <c r="O39" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="40" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>139</v>
       </c>
@@ -2963,7 +2972,7 @@
       </c>
       <c r="O40" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="41" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>139</v>
       </c>
@@ -3004,7 +3013,7 @@
       </c>
       <c r="O41" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="42" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>143</v>
       </c>
@@ -3045,7 +3054,7 @@
       </c>
       <c r="O42" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="43" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>146</v>
       </c>
@@ -3086,7 +3095,7 @@
       </c>
       <c r="O43" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="44" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>153</v>
       </c>
@@ -3127,7 +3136,7 @@
       </c>
       <c r="O44" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="45" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>161</v>
       </c>
@@ -3170,7 +3179,7 @@
       </c>
       <c r="O45" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="46" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>161</v>
       </c>
@@ -3213,7 +3222,7 @@
       </c>
       <c r="O46" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="47" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>161</v>
       </c>
@@ -3239,7 +3248,7 @@
         <v>152</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>167</v>
+        <v>291</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>50</v>
@@ -3256,7 +3265,7 @@
       </c>
       <c r="O47" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="48" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>161</v>
       </c>
@@ -3282,7 +3291,7 @@
         <v>152</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>134</v>
@@ -3299,59 +3308,59 @@
       </c>
       <c r="O48" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="49" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O49" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="50" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>150</v>
@@ -3364,7 +3373,7 @@
         <v>152</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>25</v>
@@ -3381,21 +3390,21 @@
       </c>
       <c r="O50" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="51" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2" t="s">
@@ -3411,73 +3420,73 @@
         <v>50</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="N51" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="O51" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="I52" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O52" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="53" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
@@ -3487,38 +3496,38 @@
         <v>152</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O53" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="54" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2" t="s">
@@ -3528,35 +3537,35 @@
         <v>159</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>113</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O54" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="55" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>150</v>
@@ -3586,31 +3595,31 @@
       </c>
       <c r="O55" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="56" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="I56" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>134</v>
@@ -3627,31 +3636,31 @@
       </c>
       <c r="O56" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="57" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="I57" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J57" s="2" t="s">
         <v>134</v>
@@ -3668,21 +3677,21 @@
       </c>
       <c r="O57" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="58" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2" t="s">
@@ -3692,38 +3701,38 @@
         <v>152</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>31</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L58" s="3"/>
       <c r="M58" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O58" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="59" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2" t="s">
@@ -3739,73 +3748,73 @@
         <v>41</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N59" s="3" t="s">
         <v>32</v>
       </c>
       <c r="O59" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="60" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="I60" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L60" s="3"/>
       <c r="M60" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O60" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="61" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2" t="s">
@@ -3815,38 +3824,38 @@
         <v>152</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>50</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L61" s="3"/>
       <c r="M61" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O61" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="62" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2" t="s">
@@ -3856,38 +3865,38 @@
         <v>159</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K62" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L62" s="3"/>
       <c r="M62" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O62" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="63" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2" t="s">
@@ -3903,32 +3912,32 @@
         <v>22</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L63" s="3"/>
       <c r="M63" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O63" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="64" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="E64" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2" t="s">
@@ -3938,45 +3947,45 @@
         <v>152</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>113</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L64" s="3"/>
       <c r="M64" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O64" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="65" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>121</v>
@@ -3985,29 +3994,29 @@
         <v>122</v>
       </c>
       <c r="K65" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L65" s="3"/>
       <c r="M65" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="N65" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="O65" s="2"/>
+    </row>
+    <row r="66" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="N65" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="O65" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A66" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>18</v>
@@ -4020,7 +4029,7 @@
         <v>152</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J66" s="2" t="s">
         <v>134</v>
@@ -4037,18 +4046,18 @@
       </c>
       <c r="O66" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="67" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>18</v>
@@ -4061,7 +4070,7 @@
         <v>152</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>113</v>
@@ -4078,21 +4087,21 @@
       </c>
       <c r="O67" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="68" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
@@ -4108,39 +4117,39 @@
         <v>31</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L68" s="3"/>
       <c r="M68" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="O68" s="2"/>
+    </row>
+    <row r="69" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="N68" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="O68" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A69" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>44</v>
@@ -4149,29 +4158,29 @@
         <v>41</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L69" s="3"/>
       <c r="M69" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N69" s="3" t="s">
         <v>32</v>
       </c>
       <c r="O69" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="70" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>87</v>
@@ -4201,18 +4210,18 @@
       </c>
       <c r="O70" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="71" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>87</v>
@@ -4242,18 +4251,18 @@
       </c>
       <c r="O71" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="72" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>87</v>
@@ -4266,7 +4275,7 @@
         <v>152</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J72" s="2" t="s">
         <v>113</v>
@@ -4283,18 +4292,18 @@
       </c>
       <c r="O72" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="73" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>87</v>
@@ -4307,7 +4316,7 @@
         <v>152</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>134</v>
@@ -4324,21 +4333,21 @@
       </c>
       <c r="O73" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row r="74" spans="1:15" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>273</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2" t="s">
@@ -4354,32 +4363,32 @@
         <v>50</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L74" s="3"/>
       <c r="M74" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N74" s="3" t="s">
         <v>32</v>
       </c>
       <c r="O74" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+    <row r="75" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="C75" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="E75" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="2" t="s">
@@ -4389,48 +4398,48 @@
         <v>152</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J75" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L75" s="5"/>
       <c r="M75" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N75" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="O75" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+    <row r="76" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="C76" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H76" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H76" s="6" t="s">
-        <v>175</v>
-      </c>
       <c r="I76" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>113</v>
@@ -4447,28 +4456,28 @@
       </c>
       <c r="O76" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row r="77" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="C77" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H77" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>104</v>
@@ -4488,31 +4497,31 @@
       </c>
       <c r="O77" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row r="78" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="C78" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H78" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H78" s="6" t="s">
+      <c r="I78" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="J78" s="2" t="s">
         <v>25</v>
@@ -4529,24 +4538,24 @@
       </c>
       <c r="O78" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="79" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>151</v>
@@ -4555,24 +4564,24 @@
         <v>152</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>122</v>
       </c>
       <c r="K79" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L79" s="3"/>
       <c r="M79" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N79" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O79" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="80" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4589,7 +4598,7 @@
       <c r="N80" s="3"/>
       <c r="O80" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="81" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4606,7 +4615,7 @@
       <c r="N81" s="3"/>
       <c r="O81" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="82" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4623,7 +4632,7 @@
       <c r="N82" s="3"/>
       <c r="O82" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="83" spans="1:15" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>

</xml_diff>

<commit_message>
04/07 fin journée SCB
</commit_message>
<xml_diff>
--- a/tests/fichier_test/e_e_p.xlsx
+++ b/tests/fichier_test/e_e_p.xlsx
@@ -1293,8 +1293,8 @@
   </sheetPr>
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>